<commit_message>
Revising Data and names
</commit_message>
<xml_diff>
--- a/data/corvina_length_all_gears_yeartotal_2014.xlsx
+++ b/data/corvina_length_all_gears_yeartotal_2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>length_class</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Marín, B. 2015. Evaluación de los recursos pesqueros y de la veda 2014 en la zona interior del Golfo de Nicoya. Documento Técnico Nº 20 del Departamento de Investigación Pesquera de Incopesca. 51p</t>
+  </si>
+  <si>
+    <t>Fig. 16</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -412,6 +415,11 @@
     <row r="1" spans="1:1" ht="18" customHeight="1">
       <c r="A1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -428,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>